<commit_message>
Split atom PKIX.12 into 3 seprate atoms PKIX.12, PKIX.27 and PKIX.28.  Updated all the databases to reflect the split.  moved the conformance csv log rollover action to the end of the run instead of the beggining that way csv file no longer held hostage at the end of the run.
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_Production_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_Production_Cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GSA\GSA_GIT\piv-conformance-swing\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29964794-2875-42C8-B06B-E5C0DDA5620B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62B14CA-B5B2-49E2-81FC-842A64F51060}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="1560" windowWidth="26025" windowHeight="14550" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3637" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="1264">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3817,6 +3817,18 @@
   </si>
   <si>
     <t>11.7.2.6.5</t>
+  </si>
+  <si>
+    <t>PKIX.27</t>
+  </si>
+  <si>
+    <t>PKIX_Test_27</t>
+  </si>
+  <si>
+    <t>PKIX.28</t>
+  </si>
+  <si>
+    <t>PKIX_Test_28</t>
   </si>
 </sst>
 </file>
@@ -4056,7 +4068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4254,6 +4266,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8339,10 +8357,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F466"/>
+  <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E264" sqref="E264"/>
+    <sheetView tabSelected="1" topLeftCell="A410" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A426" sqref="A426:XFD426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -14057,36 +14075,36 @@
       <c r="E347" s="39"/>
       <c r="F347" s="39"/>
     </row>
-    <row r="348" spans="1:6" ht="90">
+    <row r="348" spans="1:6" ht="60">
       <c r="A348" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B348" s="38" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C348" s="41" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D348" s="38" t="s">
-        <v>582</v>
+        <v>1260</v>
       </c>
       <c r="E348" s="38"/>
       <c r="F348" s="38" t="s">
         <v>1119</v>
       </c>
     </row>
-    <row r="349" spans="1:6" ht="60">
+    <row r="349" spans="1:6" ht="45">
       <c r="A349" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B349" s="38" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="C349" s="41" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="D349" s="38" t="s">
-        <v>582</v>
+        <v>591</v>
       </c>
       <c r="E349" s="38"/>
       <c r="F349" s="38" t="s">
@@ -14098,49 +14116,45 @@
         <v>56</v>
       </c>
       <c r="B350" s="38" t="s">
-        <v>587</v>
-      </c>
-      <c r="C350" s="38" t="s">
-        <v>588</v>
+        <v>592</v>
+      </c>
+      <c r="C350" s="41" t="s">
+        <v>593</v>
       </c>
       <c r="D350" s="38" t="s">
-        <v>1159</v>
+        <v>594</v>
       </c>
       <c r="E350" s="38"/>
       <c r="F350" s="38" t="s">
         <v>1119</v>
       </c>
     </row>
-    <row r="351" spans="1:6" ht="45">
+    <row r="351" spans="1:6">
       <c r="A351" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B351" s="38" t="s">
-        <v>589</v>
-      </c>
-      <c r="C351" s="41" t="s">
-        <v>590</v>
-      </c>
-      <c r="D351" s="38" t="s">
-        <v>591</v>
-      </c>
-      <c r="E351" s="38"/>
-      <c r="F351" s="38" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6" ht="30">
+        <v>595</v>
+      </c>
+      <c r="C351" s="39" t="s">
+        <v>596</v>
+      </c>
+      <c r="D351" s="39"/>
+      <c r="E351" s="39"/>
+      <c r="F351" s="39"/>
+    </row>
+    <row r="352" spans="1:6">
       <c r="A352" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B352" s="38" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="C352" s="41" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="D352" s="38" t="s">
-        <v>594</v>
+        <v>573</v>
       </c>
       <c r="E352" s="38"/>
       <c r="F352" s="38" t="s">
@@ -14152,97 +14166,101 @@
         <v>56</v>
       </c>
       <c r="B353" s="38" t="s">
-        <v>595</v>
-      </c>
-      <c r="C353" s="39" t="s">
-        <v>596</v>
-      </c>
-      <c r="D353" s="39"/>
-      <c r="E353" s="39"/>
-      <c r="F353" s="39"/>
+        <v>599</v>
+      </c>
+      <c r="C353" s="38" t="s">
+        <v>600</v>
+      </c>
+      <c r="D353" s="38" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E353" s="38"/>
+      <c r="F353" s="38" t="s">
+        <v>1119</v>
+      </c>
     </row>
     <row r="354" spans="1:6">
       <c r="A354" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B354" s="38" t="s">
-        <v>597</v>
-      </c>
-      <c r="C354" s="41" t="s">
-        <v>598</v>
-      </c>
-      <c r="D354" s="38" t="s">
-        <v>573</v>
-      </c>
-      <c r="E354" s="38"/>
-      <c r="F354" s="38" t="s">
-        <v>1119</v>
-      </c>
+        <v>601</v>
+      </c>
+      <c r="C354" s="39" t="s">
+        <v>602</v>
+      </c>
+      <c r="D354" s="39"/>
+      <c r="E354" s="39"/>
+      <c r="F354" s="39"/>
     </row>
     <row r="355" spans="1:6">
       <c r="A355" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B355" s="38" t="s">
-        <v>599</v>
-      </c>
-      <c r="C355" s="38" t="s">
-        <v>600</v>
+        <v>603</v>
+      </c>
+      <c r="C355" s="41" t="s">
+        <v>566</v>
       </c>
       <c r="D355" s="38" t="s">
-        <v>1059</v>
+        <v>567</v>
       </c>
       <c r="E355" s="38"/>
       <c r="F355" s="38" t="s">
         <v>1119</v>
       </c>
     </row>
-    <row r="356" spans="1:6">
+    <row r="356" spans="1:6" ht="30">
       <c r="A356" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B356" s="38" t="s">
-        <v>601</v>
-      </c>
-      <c r="C356" s="39" t="s">
-        <v>602</v>
-      </c>
-      <c r="D356" s="39"/>
-      <c r="E356" s="39"/>
-      <c r="F356" s="39"/>
-    </row>
-    <row r="357" spans="1:6">
+        <v>604</v>
+      </c>
+      <c r="C356" s="41" t="s">
+        <v>605</v>
+      </c>
+      <c r="D356" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E356" s="42"/>
+      <c r="F356" s="38" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" ht="30">
       <c r="A357" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B357" s="38" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="C357" s="41" t="s">
-        <v>566</v>
+        <v>607</v>
       </c>
       <c r="D357" s="38" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="E357" s="38"/>
       <c r="F357" s="38" t="s">
         <v>1119</v>
       </c>
     </row>
-    <row r="358" spans="1:6" ht="30">
+    <row r="358" spans="1:6">
       <c r="A358" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B358" s="38" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="C358" s="41" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="D358" s="38" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E358" s="42"/>
+        <v>1062</v>
+      </c>
+      <c r="E358" s="38"/>
       <c r="F358" s="38" t="s">
         <v>1119</v>
       </c>
@@ -14252,13 +14270,13 @@
         <v>56</v>
       </c>
       <c r="B359" s="38" t="s">
-        <v>606</v>
-      </c>
-      <c r="C359" s="41" t="s">
-        <v>607</v>
+        <v>610</v>
+      </c>
+      <c r="C359" s="38" t="s">
+        <v>611</v>
       </c>
       <c r="D359" s="38" t="s">
-        <v>573</v>
+        <v>1060</v>
       </c>
       <c r="E359" s="38"/>
       <c r="F359" s="38" t="s">
@@ -14269,196 +14287,196 @@
       <c r="A360" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B360" s="38" t="s">
-        <v>608</v>
-      </c>
-      <c r="C360" s="41" t="s">
-        <v>609</v>
-      </c>
-      <c r="D360" s="38" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E360" s="38"/>
-      <c r="F360" s="38" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="361" spans="1:6" ht="30">
+      <c r="B360" s="38">
+        <v>11.2</v>
+      </c>
+      <c r="C360" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D360" s="39"/>
+      <c r="E360" s="39"/>
+      <c r="F360" s="39"/>
+    </row>
+    <row r="361" spans="1:6">
       <c r="A361" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B361" s="38" t="s">
-        <v>610</v>
-      </c>
-      <c r="C361" s="38" t="s">
-        <v>611</v>
-      </c>
-      <c r="D361" s="38" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E361" s="38"/>
-      <c r="F361" s="38" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6">
+        <v>612</v>
+      </c>
+      <c r="C361" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D361" s="39"/>
+      <c r="E361" s="39"/>
+      <c r="F361" s="39"/>
+    </row>
+    <row r="362" spans="1:6" ht="120">
       <c r="A362" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B362" s="38">
-        <v>11.2</v>
-      </c>
-      <c r="C362" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D362" s="39"/>
-      <c r="E362" s="39"/>
-      <c r="F362" s="39"/>
-    </row>
-    <row r="363" spans="1:6">
+      <c r="B362" s="38" t="s">
+        <v>613</v>
+      </c>
+      <c r="C362" s="41" t="s">
+        <v>545</v>
+      </c>
+      <c r="D362" s="38" t="s">
+        <v>998</v>
+      </c>
+      <c r="E362" s="38"/>
+      <c r="F362" s="38" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" ht="30">
       <c r="A363" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B363" s="38" t="s">
-        <v>612</v>
-      </c>
-      <c r="C363" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D363" s="39"/>
-      <c r="E363" s="39"/>
-      <c r="F363" s="39"/>
-    </row>
-    <row r="364" spans="1:6" ht="120">
+        <v>614</v>
+      </c>
+      <c r="C363" s="41" t="s">
+        <v>615</v>
+      </c>
+      <c r="D363" s="38" t="s">
+        <v>993</v>
+      </c>
+      <c r="E363" s="38"/>
+      <c r="F363" s="38" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" ht="30">
       <c r="A364" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B364" s="38" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="C364" s="41" t="s">
-        <v>545</v>
-      </c>
-      <c r="D364" s="38" t="s">
-        <v>998</v>
+        <v>549</v>
+      </c>
+      <c r="D364" s="38">
+        <v>78.099999999999994</v>
       </c>
       <c r="E364" s="38"/>
       <c r="F364" s="38" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="365" spans="1:6" ht="30">
+    <row r="365" spans="1:6">
       <c r="A365" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B365" s="38" t="s">
-        <v>614</v>
-      </c>
-      <c r="C365" s="41" t="s">
-        <v>615</v>
-      </c>
-      <c r="D365" s="38" t="s">
-        <v>993</v>
-      </c>
-      <c r="E365" s="38"/>
-      <c r="F365" s="38" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6" ht="30">
+        <v>617</v>
+      </c>
+      <c r="C365" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D365" s="39"/>
+      <c r="E365" s="39"/>
+      <c r="F365" s="39"/>
+    </row>
+    <row r="366" spans="1:6">
       <c r="A366" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B366" s="38" t="s">
-        <v>616</v>
-      </c>
-      <c r="C366" s="41" t="s">
-        <v>549</v>
-      </c>
-      <c r="D366" s="38">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E366" s="38"/>
-      <c r="F366" s="38" t="s">
-        <v>1137</v>
-      </c>
+        <v>618</v>
+      </c>
+      <c r="C366" s="39" t="s">
+        <v>619</v>
+      </c>
+      <c r="D366" s="39"/>
+      <c r="E366" s="39"/>
+      <c r="F366" s="39"/>
     </row>
     <row r="367" spans="1:6">
       <c r="A367" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B367" s="38" t="s">
-        <v>617</v>
-      </c>
-      <c r="C367" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D367" s="39"/>
-      <c r="E367" s="39"/>
-      <c r="F367" s="39"/>
-    </row>
-    <row r="368" spans="1:6">
+        <v>620</v>
+      </c>
+      <c r="C367" s="38" t="s">
+        <v>621</v>
+      </c>
+      <c r="D367" s="38" t="s">
+        <v>622</v>
+      </c>
+      <c r="E367" s="38"/>
+      <c r="F367" s="38" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" ht="30">
       <c r="A368" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B368" s="38" t="s">
-        <v>618</v>
-      </c>
-      <c r="C368" s="39" t="s">
-        <v>619</v>
-      </c>
-      <c r="D368" s="39"/>
-      <c r="E368" s="39"/>
-      <c r="F368" s="39"/>
-    </row>
-    <row r="369" spans="1:6">
+        <v>623</v>
+      </c>
+      <c r="C368" s="41" t="s">
+        <v>624</v>
+      </c>
+      <c r="D368" s="38" t="s">
+        <v>625</v>
+      </c>
+      <c r="E368" s="38"/>
+      <c r="F368" s="38" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" ht="45">
       <c r="A369" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B369" s="38" t="s">
-        <v>620</v>
-      </c>
-      <c r="C369" s="38" t="s">
-        <v>621</v>
+        <v>626</v>
+      </c>
+      <c r="C369" s="41" t="s">
+        <v>627</v>
       </c>
       <c r="D369" s="38" t="s">
-        <v>622</v>
+        <v>579</v>
       </c>
       <c r="E369" s="38"/>
       <c r="F369" s="38" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="370" spans="1:6" ht="30">
+    <row r="370" spans="1:6" ht="45">
       <c r="A370" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B370" s="38" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="C370" s="41" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="D370" s="38" t="s">
-        <v>625</v>
+        <v>591</v>
       </c>
       <c r="E370" s="38"/>
       <c r="F370" s="38" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="371" spans="1:6" ht="45">
+    <row r="371" spans="1:6" ht="30">
       <c r="A371" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B371" s="38" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="C371" s="41" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="D371" s="38" t="s">
-        <v>579</v>
+        <v>594</v>
       </c>
       <c r="E371" s="38"/>
       <c r="F371" s="38" t="s">
@@ -14470,49 +14488,45 @@
         <v>56</v>
       </c>
       <c r="B372" s="38" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="C372" s="41" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="D372" s="38" t="s">
-        <v>591</v>
+        <v>562</v>
       </c>
       <c r="E372" s="38"/>
       <c r="F372" s="38" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="30">
+    <row r="373" spans="1:6">
       <c r="A373" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B373" s="38" t="s">
-        <v>630</v>
-      </c>
-      <c r="C373" s="41" t="s">
-        <v>631</v>
-      </c>
-      <c r="D373" s="38" t="s">
-        <v>594</v>
-      </c>
-      <c r="E373" s="38"/>
-      <c r="F373" s="38" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="374" spans="1:6" ht="45">
+        <v>634</v>
+      </c>
+      <c r="C373" s="39" t="s">
+        <v>596</v>
+      </c>
+      <c r="D373" s="39"/>
+      <c r="E373" s="39"/>
+      <c r="F373" s="39"/>
+    </row>
+    <row r="374" spans="1:6">
       <c r="A374" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B374" s="38" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="C374" s="41" t="s">
-        <v>633</v>
+        <v>598</v>
       </c>
       <c r="D374" s="38" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="E374" s="38"/>
       <c r="F374" s="38" t="s">
@@ -14524,97 +14538,101 @@
         <v>56</v>
       </c>
       <c r="B375" s="38" t="s">
-        <v>634</v>
-      </c>
-      <c r="C375" s="39" t="s">
-        <v>596</v>
-      </c>
-      <c r="D375" s="39"/>
-      <c r="E375" s="39"/>
-      <c r="F375" s="39"/>
+        <v>636</v>
+      </c>
+      <c r="C375" s="38" t="s">
+        <v>600</v>
+      </c>
+      <c r="D375" s="38" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E375" s="38"/>
+      <c r="F375" s="38" t="s">
+        <v>1137</v>
+      </c>
     </row>
     <row r="376" spans="1:6">
       <c r="A376" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B376" s="38" t="s">
-        <v>635</v>
-      </c>
-      <c r="C376" s="41" t="s">
-        <v>598</v>
-      </c>
-      <c r="D376" s="38" t="s">
-        <v>573</v>
-      </c>
-      <c r="E376" s="38"/>
-      <c r="F376" s="38" t="s">
-        <v>1137</v>
-      </c>
+        <v>637</v>
+      </c>
+      <c r="C376" s="39" t="s">
+        <v>602</v>
+      </c>
+      <c r="D376" s="39"/>
+      <c r="E376" s="39"/>
+      <c r="F376" s="39"/>
     </row>
     <row r="377" spans="1:6">
       <c r="A377" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B377" s="38" t="s">
-        <v>636</v>
-      </c>
-      <c r="C377" s="38" t="s">
-        <v>600</v>
+        <v>638</v>
+      </c>
+      <c r="C377" s="41" t="s">
+        <v>566</v>
       </c>
       <c r="D377" s="38" t="s">
-        <v>1059</v>
+        <v>567</v>
       </c>
       <c r="E377" s="38"/>
       <c r="F377" s="38" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="378" spans="1:6">
+    <row r="378" spans="1:6" ht="30">
       <c r="A378" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B378" s="38" t="s">
-        <v>637</v>
-      </c>
-      <c r="C378" s="39" t="s">
-        <v>602</v>
-      </c>
-      <c r="D378" s="39"/>
-      <c r="E378" s="39"/>
-      <c r="F378" s="39"/>
-    </row>
-    <row r="379" spans="1:6">
+        <v>639</v>
+      </c>
+      <c r="C378" s="41" t="s">
+        <v>640</v>
+      </c>
+      <c r="D378" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E378" s="42"/>
+      <c r="F378" s="38" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" ht="30">
       <c r="A379" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B379" s="38" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="C379" s="41" t="s">
-        <v>566</v>
+        <v>607</v>
       </c>
       <c r="D379" s="38" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="E379" s="38"/>
       <c r="F379" s="38" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="30">
+    <row r="380" spans="1:6">
       <c r="A380" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B380" s="38" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="C380" s="41" t="s">
-        <v>640</v>
+        <v>609</v>
       </c>
       <c r="D380" s="38" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E380" s="42"/>
+        <v>1062</v>
+      </c>
+      <c r="E380" s="38"/>
       <c r="F380" s="38" t="s">
         <v>1137</v>
       </c>
@@ -14624,13 +14642,13 @@
         <v>56</v>
       </c>
       <c r="B381" s="38" t="s">
-        <v>641</v>
-      </c>
-      <c r="C381" s="41" t="s">
-        <v>607</v>
+        <v>643</v>
+      </c>
+      <c r="C381" s="38" t="s">
+        <v>611</v>
       </c>
       <c r="D381" s="38" t="s">
-        <v>573</v>
+        <v>1060</v>
       </c>
       <c r="E381" s="38"/>
       <c r="F381" s="38" t="s">
@@ -14641,160 +14659,160 @@
       <c r="A382" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B382" s="38" t="s">
-        <v>642</v>
-      </c>
-      <c r="C382" s="41" t="s">
-        <v>609</v>
-      </c>
-      <c r="D382" s="38" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E382" s="38"/>
-      <c r="F382" s="38" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="383" spans="1:6" ht="30">
+      <c r="B382" s="38">
+        <v>11.3</v>
+      </c>
+      <c r="C382" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D382" s="39"/>
+      <c r="E382" s="39"/>
+      <c r="F382" s="39"/>
+    </row>
+    <row r="383" spans="1:6">
       <c r="A383" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B383" s="38" t="s">
-        <v>643</v>
-      </c>
-      <c r="C383" s="38" t="s">
-        <v>611</v>
-      </c>
-      <c r="D383" s="38" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E383" s="38"/>
-      <c r="F383" s="38" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6">
+        <v>644</v>
+      </c>
+      <c r="C383" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D383" s="39"/>
+      <c r="E383" s="39"/>
+      <c r="F383" s="39"/>
+    </row>
+    <row r="384" spans="1:6" ht="105">
       <c r="A384" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B384" s="38">
-        <v>11.3</v>
-      </c>
-      <c r="C384" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D384" s="39"/>
-      <c r="E384" s="39"/>
-      <c r="F384" s="39"/>
-    </row>
-    <row r="385" spans="1:6">
+      <c r="B384" s="38" t="s">
+        <v>645</v>
+      </c>
+      <c r="C384" s="41" t="s">
+        <v>646</v>
+      </c>
+      <c r="D384" s="38">
+        <v>78.3</v>
+      </c>
+      <c r="E384" s="38"/>
+      <c r="F384" s="38" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" ht="30">
       <c r="A385" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B385" s="38" t="s">
-        <v>644</v>
-      </c>
-      <c r="C385" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D385" s="39"/>
-      <c r="E385" s="39"/>
-      <c r="F385" s="39"/>
-    </row>
-    <row r="386" spans="1:6" ht="105">
+        <v>647</v>
+      </c>
+      <c r="C385" s="38" t="s">
+        <v>648</v>
+      </c>
+      <c r="D385" s="38" t="s">
+        <v>993</v>
+      </c>
+      <c r="E385" s="38"/>
+      <c r="F385" s="38" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" ht="30">
       <c r="A386" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B386" s="38" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="C386" s="41" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="D386" s="38">
-        <v>78.3</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E386" s="38"/>
       <c r="F386" s="38" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="387" spans="1:6" ht="30">
+    <row r="387" spans="1:6">
       <c r="A387" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B387" s="38" t="s">
-        <v>647</v>
-      </c>
-      <c r="C387" s="38" t="s">
-        <v>648</v>
-      </c>
-      <c r="D387" s="38" t="s">
-        <v>993</v>
-      </c>
-      <c r="E387" s="38"/>
-      <c r="F387" s="38" t="s">
+        <v>651</v>
+      </c>
+      <c r="C387" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D387" s="39"/>
+      <c r="E387" s="39"/>
+      <c r="F387" s="39"/>
+    </row>
+    <row r="388" spans="1:6">
+      <c r="A388" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B388" s="38" t="s">
+        <v>652</v>
+      </c>
+      <c r="C388" s="39" t="s">
+        <v>619</v>
+      </c>
+      <c r="D388" s="39"/>
+      <c r="E388" s="39"/>
+      <c r="F388" s="39"/>
+    </row>
+    <row r="389" spans="1:6" ht="45">
+      <c r="A389" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B389" s="38" t="s">
+        <v>653</v>
+      </c>
+      <c r="C389" s="41" t="s">
+        <v>654</v>
+      </c>
+      <c r="D389" s="38" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E389" s="38"/>
+      <c r="F389" s="38" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="388" spans="1:6" ht="30">
-      <c r="A388" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B388" s="38" t="s">
-        <v>649</v>
-      </c>
-      <c r="C388" s="41" t="s">
-        <v>650</v>
-      </c>
-      <c r="D388" s="38">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E388" s="38"/>
-      <c r="F388" s="38" t="s">
+    <row r="390" spans="1:6" ht="45">
+      <c r="A390" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B390" s="38" t="s">
+        <v>655</v>
+      </c>
+      <c r="C390" s="41" t="s">
+        <v>656</v>
+      </c>
+      <c r="D390" s="38" t="s">
+        <v>657</v>
+      </c>
+      <c r="E390" s="38"/>
+      <c r="F390" s="38" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="389" spans="1:6">
-      <c r="A389" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B389" s="38" t="s">
-        <v>651</v>
-      </c>
-      <c r="C389" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D389" s="39"/>
-      <c r="E389" s="39"/>
-      <c r="F389" s="39"/>
-    </row>
-    <row r="390" spans="1:6">
-      <c r="A390" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B390" s="38" t="s">
-        <v>652</v>
-      </c>
-      <c r="C390" s="39" t="s">
-        <v>619</v>
-      </c>
-      <c r="D390" s="39"/>
-      <c r="E390" s="39"/>
-      <c r="F390" s="39"/>
-    </row>
-    <row r="391" spans="1:6" ht="45">
+    <row r="391" spans="1:6">
       <c r="A391" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B391" s="38" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
       <c r="C391" s="41" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="D391" s="38" t="s">
-        <v>1031</v>
+        <v>556</v>
       </c>
       <c r="E391" s="38"/>
       <c r="F391" s="38" t="s">
@@ -14806,31 +14824,31 @@
         <v>56</v>
       </c>
       <c r="B392" s="38" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C392" s="41" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="D392" s="38" t="s">
-        <v>657</v>
+        <v>579</v>
       </c>
       <c r="E392" s="38"/>
       <c r="F392" s="38" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="393" spans="1:6">
+    <row r="393" spans="1:6" ht="30">
       <c r="A393" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B393" s="38" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="C393" s="41" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="D393" s="38" t="s">
-        <v>556</v>
+        <v>594</v>
       </c>
       <c r="E393" s="38"/>
       <c r="F393" s="38" t="s">
@@ -14842,49 +14860,45 @@
         <v>56</v>
       </c>
       <c r="B394" s="38" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="C394" s="41" t="s">
-        <v>661</v>
+        <v>633</v>
       </c>
       <c r="D394" s="38" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
       <c r="E394" s="38"/>
       <c r="F394" s="38" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="395" spans="1:6" ht="30">
+    <row r="395" spans="1:6">
       <c r="A395" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B395" s="38" t="s">
-        <v>662</v>
-      </c>
-      <c r="C395" s="41" t="s">
-        <v>663</v>
-      </c>
-      <c r="D395" s="38" t="s">
-        <v>594</v>
-      </c>
-      <c r="E395" s="38"/>
-      <c r="F395" s="38" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6" ht="45">
+        <v>665</v>
+      </c>
+      <c r="C395" s="39" t="s">
+        <v>596</v>
+      </c>
+      <c r="D395" s="39"/>
+      <c r="E395" s="39"/>
+      <c r="F395" s="39"/>
+    </row>
+    <row r="396" spans="1:6">
       <c r="A396" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B396" s="38" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="C396" s="41" t="s">
-        <v>633</v>
+        <v>598</v>
       </c>
       <c r="D396" s="38" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="E396" s="38"/>
       <c r="F396" s="38" t="s">
@@ -14896,97 +14910,101 @@
         <v>56</v>
       </c>
       <c r="B397" s="38" t="s">
-        <v>665</v>
-      </c>
-      <c r="C397" s="39" t="s">
-        <v>596</v>
-      </c>
-      <c r="D397" s="39"/>
-      <c r="E397" s="39"/>
-      <c r="F397" s="39"/>
+        <v>667</v>
+      </c>
+      <c r="C397" s="38" t="s">
+        <v>600</v>
+      </c>
+      <c r="D397" s="38" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E397" s="38"/>
+      <c r="F397" s="38" t="s">
+        <v>1140</v>
+      </c>
     </row>
     <row r="398" spans="1:6">
       <c r="A398" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B398" s="38" t="s">
-        <v>666</v>
-      </c>
-      <c r="C398" s="41" t="s">
-        <v>598</v>
-      </c>
-      <c r="D398" s="38" t="s">
-        <v>573</v>
-      </c>
-      <c r="E398" s="38"/>
-      <c r="F398" s="38" t="s">
-        <v>1140</v>
-      </c>
+        <v>668</v>
+      </c>
+      <c r="C398" s="39" t="s">
+        <v>602</v>
+      </c>
+      <c r="D398" s="39"/>
+      <c r="E398" s="39"/>
+      <c r="F398" s="39"/>
     </row>
     <row r="399" spans="1:6">
       <c r="A399" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B399" s="38" t="s">
-        <v>667</v>
-      </c>
-      <c r="C399" s="38" t="s">
-        <v>600</v>
+        <v>669</v>
+      </c>
+      <c r="C399" s="41" t="s">
+        <v>566</v>
       </c>
       <c r="D399" s="38" t="s">
-        <v>1059</v>
+        <v>567</v>
       </c>
       <c r="E399" s="38"/>
       <c r="F399" s="38" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="400" spans="1:6">
+    <row r="400" spans="1:6" ht="30">
       <c r="A400" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B400" s="38" t="s">
-        <v>668</v>
-      </c>
-      <c r="C400" s="39" t="s">
-        <v>602</v>
-      </c>
-      <c r="D400" s="39"/>
-      <c r="E400" s="39"/>
-      <c r="F400" s="39"/>
-    </row>
-    <row r="401" spans="1:6">
+        <v>670</v>
+      </c>
+      <c r="C400" s="41" t="s">
+        <v>640</v>
+      </c>
+      <c r="D400" s="38" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E400" s="42"/>
+      <c r="F400" s="38" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" ht="30">
       <c r="A401" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B401" s="38" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="C401" s="41" t="s">
-        <v>566</v>
+        <v>607</v>
       </c>
       <c r="D401" s="38" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="E401" s="38"/>
       <c r="F401" s="38" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="30">
+    <row r="402" spans="1:6">
       <c r="A402" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B402" s="38" t="s">
-        <v>670</v>
-      </c>
-      <c r="C402" s="41" t="s">
-        <v>640</v>
+        <v>672</v>
+      </c>
+      <c r="C402" s="38" t="s">
+        <v>609</v>
       </c>
       <c r="D402" s="38" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E402" s="42"/>
+        <v>1062</v>
+      </c>
+      <c r="E402" s="38"/>
       <c r="F402" s="38" t="s">
         <v>1140</v>
       </c>
@@ -14996,13 +15014,13 @@
         <v>56</v>
       </c>
       <c r="B403" s="38" t="s">
-        <v>671</v>
-      </c>
-      <c r="C403" s="41" t="s">
-        <v>607</v>
+        <v>673</v>
+      </c>
+      <c r="C403" s="38" t="s">
+        <v>611</v>
       </c>
       <c r="D403" s="38" t="s">
-        <v>573</v>
+        <v>1060</v>
       </c>
       <c r="E403" s="38"/>
       <c r="F403" s="38" t="s">
@@ -15013,178 +15031,178 @@
       <c r="A404" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B404" s="38" t="s">
-        <v>672</v>
-      </c>
-      <c r="C404" s="38" t="s">
-        <v>609</v>
-      </c>
-      <c r="D404" s="38" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E404" s="38"/>
-      <c r="F404" s="38" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="405" spans="1:6" ht="30">
+      <c r="B404" s="38">
+        <v>11.4</v>
+      </c>
+      <c r="C404" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D404" s="39"/>
+      <c r="E404" s="39"/>
+      <c r="F404" s="39"/>
+    </row>
+    <row r="405" spans="1:6">
       <c r="A405" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B405" s="38" t="s">
-        <v>673</v>
-      </c>
-      <c r="C405" s="38" t="s">
-        <v>611</v>
-      </c>
-      <c r="D405" s="38" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E405" s="38"/>
-      <c r="F405" s="38" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="406" spans="1:6">
+        <v>674</v>
+      </c>
+      <c r="C405" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D405" s="39"/>
+      <c r="E405" s="39"/>
+      <c r="F405" s="39"/>
+    </row>
+    <row r="406" spans="1:6" ht="105">
       <c r="A406" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B406" s="38">
-        <v>11.4</v>
-      </c>
-      <c r="C406" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="D406" s="39"/>
-      <c r="E406" s="39"/>
-      <c r="F406" s="39"/>
-    </row>
-    <row r="407" spans="1:6">
+      <c r="B406" s="38" t="s">
+        <v>675</v>
+      </c>
+      <c r="C406" s="41" t="s">
+        <v>646</v>
+      </c>
+      <c r="D406" s="38">
+        <v>78.3</v>
+      </c>
+      <c r="E406" s="6"/>
+      <c r="F406" s="38" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" ht="30">
       <c r="A407" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B407" s="38" t="s">
-        <v>674</v>
-      </c>
-      <c r="C407" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D407" s="39"/>
-      <c r="E407" s="39"/>
-      <c r="F407" s="39"/>
-    </row>
-    <row r="408" spans="1:6" ht="105">
+        <v>676</v>
+      </c>
+      <c r="C407" s="41" t="s">
+        <v>677</v>
+      </c>
+      <c r="D407" s="38">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E407" s="38"/>
+      <c r="F407" s="38" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" ht="30">
       <c r="A408" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B408" s="38" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="C408" s="41" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="D408" s="38">
-        <v>78.3</v>
-      </c>
-      <c r="E408" s="6"/>
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E408" s="38"/>
       <c r="F408" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="409" spans="1:6" ht="30">
+    <row r="409" spans="1:6">
       <c r="A409" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B409" s="38" t="s">
-        <v>676</v>
-      </c>
-      <c r="C409" s="41" t="s">
-        <v>677</v>
-      </c>
-      <c r="D409" s="38">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E409" s="38"/>
-      <c r="F409" s="38" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6" ht="30">
+        <v>679</v>
+      </c>
+      <c r="C409" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D409" s="39"/>
+      <c r="E409" s="39"/>
+      <c r="F409" s="39"/>
+    </row>
+    <row r="410" spans="1:6">
       <c r="A410" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B410" s="38" t="s">
-        <v>678</v>
-      </c>
-      <c r="C410" s="41" t="s">
-        <v>650</v>
-      </c>
-      <c r="D410" s="38">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E410" s="38"/>
-      <c r="F410" s="38" t="s">
-        <v>1143</v>
-      </c>
+        <v>680</v>
+      </c>
+      <c r="C410" s="39" t="s">
+        <v>619</v>
+      </c>
+      <c r="D410" s="39"/>
+      <c r="E410" s="39"/>
+      <c r="F410" s="39"/>
     </row>
     <row r="411" spans="1:6">
       <c r="A411" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B411" s="38" t="s">
-        <v>679</v>
-      </c>
-      <c r="C411" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D411" s="39"/>
-      <c r="E411" s="39"/>
-      <c r="F411" s="39"/>
+        <v>681</v>
+      </c>
+      <c r="C411" s="38" t="s">
+        <v>621</v>
+      </c>
+      <c r="D411" s="38" t="s">
+        <v>622</v>
+      </c>
+      <c r="E411" s="38"/>
+      <c r="F411" s="38" t="s">
+        <v>1143</v>
+      </c>
     </row>
     <row r="412" spans="1:6">
       <c r="A412" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B412" s="38" t="s">
-        <v>680</v>
-      </c>
-      <c r="C412" s="39" t="s">
-        <v>619</v>
-      </c>
-      <c r="D412" s="39"/>
-      <c r="E412" s="39"/>
-      <c r="F412" s="39"/>
+        <v>682</v>
+      </c>
+      <c r="C412" s="41" t="s">
+        <v>683</v>
+      </c>
+      <c r="D412" s="38" t="s">
+        <v>553</v>
+      </c>
+      <c r="E412" s="38"/>
+      <c r="F412" s="38" t="s">
+        <v>1143</v>
+      </c>
     </row>
     <row r="413" spans="1:6">
       <c r="A413" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B413" s="38" t="s">
-        <v>681</v>
-      </c>
-      <c r="C413" s="38" t="s">
-        <v>621</v>
+        <v>684</v>
+      </c>
+      <c r="C413" s="41" t="s">
+        <v>685</v>
       </c>
       <c r="D413" s="38" t="s">
-        <v>622</v>
+        <v>556</v>
       </c>
       <c r="E413" s="38"/>
       <c r="F413" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="414" spans="1:6">
+    <row r="414" spans="1:6" ht="30">
       <c r="A414" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B414" s="38" t="s">
-        <v>682</v>
-      </c>
-      <c r="C414" s="41" t="s">
-        <v>683</v>
+        <v>686</v>
+      </c>
+      <c r="C414" s="38" t="s">
+        <v>687</v>
       </c>
       <c r="D414" s="38" t="s">
-        <v>553</v>
+        <v>562</v>
       </c>
       <c r="E414" s="38"/>
       <c r="F414" s="38" t="s">
@@ -15196,99 +15214,95 @@
         <v>56</v>
       </c>
       <c r="B415" s="38" t="s">
-        <v>684</v>
-      </c>
-      <c r="C415" s="41" t="s">
-        <v>685</v>
-      </c>
-      <c r="D415" s="38" t="s">
-        <v>556</v>
-      </c>
-      <c r="E415" s="38"/>
-      <c r="F415" s="38" t="s">
-        <v>1143</v>
-      </c>
+        <v>688</v>
+      </c>
+      <c r="C415" s="39" t="s">
+        <v>689</v>
+      </c>
+      <c r="D415" s="39"/>
+      <c r="E415" s="39"/>
+      <c r="F415" s="39"/>
     </row>
     <row r="416" spans="1:6" ht="30">
       <c r="A416" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B416" s="38" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="C416" s="38" t="s">
-        <v>687</v>
+        <v>1239</v>
       </c>
       <c r="D416" s="38" t="s">
-        <v>562</v>
+        <v>692</v>
       </c>
       <c r="E416" s="38"/>
       <c r="F416" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="417" spans="1:6">
+    <row r="417" spans="1:6" ht="30">
       <c r="A417" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B417" s="38" t="s">
-        <v>688</v>
-      </c>
-      <c r="C417" s="39" t="s">
-        <v>689</v>
-      </c>
-      <c r="D417" s="39"/>
-      <c r="E417" s="39"/>
-      <c r="F417" s="39"/>
+        <v>693</v>
+      </c>
+      <c r="C417" s="38" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D417" s="38" t="s">
+        <v>695</v>
+      </c>
+      <c r="E417" s="38"/>
+      <c r="F417" s="38" t="s">
+        <v>1143</v>
+      </c>
     </row>
     <row r="418" spans="1:6" ht="30">
       <c r="A418" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B418" s="38" t="s">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="C418" s="38" t="s">
-        <v>1239</v>
+        <v>697</v>
       </c>
       <c r="D418" s="38" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="E418" s="38"/>
       <c r="F418" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="30">
+    <row r="419" spans="1:6">
       <c r="A419" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B419" s="38" t="s">
-        <v>693</v>
-      </c>
-      <c r="C419" s="38" t="s">
-        <v>1240</v>
-      </c>
-      <c r="D419" s="38" t="s">
-        <v>695</v>
-      </c>
-      <c r="E419" s="38"/>
-      <c r="F419" s="38" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="420" spans="1:6" ht="30">
+        <v>698</v>
+      </c>
+      <c r="C419" s="39" t="s">
+        <v>602</v>
+      </c>
+      <c r="D419" s="39"/>
+      <c r="E419" s="39"/>
+      <c r="F419" s="39"/>
+    </row>
+    <row r="420" spans="1:6">
       <c r="A420" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B420" s="38" t="s">
-        <v>696</v>
-      </c>
-      <c r="C420" s="38" t="s">
-        <v>697</v>
+        <v>699</v>
+      </c>
+      <c r="C420" s="41" t="s">
+        <v>566</v>
       </c>
       <c r="D420" s="38" t="s">
-        <v>695</v>
+        <v>567</v>
       </c>
       <c r="E420" s="38"/>
       <c r="F420" s="38" t="s">
@@ -15300,27 +15314,31 @@
         <v>56</v>
       </c>
       <c r="B421" s="38" t="s">
-        <v>698</v>
-      </c>
-      <c r="C421" s="39" t="s">
-        <v>602</v>
-      </c>
-      <c r="D421" s="39"/>
-      <c r="E421" s="39"/>
-      <c r="F421" s="39"/>
-    </row>
-    <row r="422" spans="1:6">
+        <v>700</v>
+      </c>
+      <c r="C421" s="41" t="s">
+        <v>701</v>
+      </c>
+      <c r="D421" s="38" t="s">
+        <v>570</v>
+      </c>
+      <c r="E421" s="38"/>
+      <c r="F421" s="38" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" ht="30">
       <c r="A422" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B422" s="38" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="C422" s="41" t="s">
-        <v>566</v>
+        <v>607</v>
       </c>
       <c r="D422" s="38" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="E422" s="38"/>
       <c r="F422" s="38" t="s">
@@ -15332,31 +15350,31 @@
         <v>56</v>
       </c>
       <c r="B423" s="38" t="s">
-        <v>700</v>
-      </c>
-      <c r="C423" s="41" t="s">
-        <v>701</v>
+        <v>703</v>
+      </c>
+      <c r="C423" s="38" t="s">
+        <v>609</v>
       </c>
       <c r="D423" s="38" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="E423" s="38"/>
       <c r="F423" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="424" spans="1:6" ht="30">
+    <row r="424" spans="1:6" ht="45">
       <c r="A424" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B424" s="38" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="C424" s="41" t="s">
-        <v>607</v>
+        <v>661</v>
       </c>
       <c r="D424" s="38" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="E424" s="38"/>
       <c r="F424" s="38" t="s">
@@ -15368,117 +15386,113 @@
         <v>56</v>
       </c>
       <c r="B425" s="38" t="s">
-        <v>703</v>
-      </c>
-      <c r="C425" s="38" t="s">
-        <v>609</v>
-      </c>
-      <c r="D425" s="38" t="s">
-        <v>573</v>
-      </c>
-      <c r="E425" s="38"/>
-      <c r="F425" s="38" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="426" spans="1:6" ht="45">
+        <v>706</v>
+      </c>
+      <c r="C425" s="39" t="s">
+        <v>581</v>
+      </c>
+      <c r="D425" s="39"/>
+      <c r="E425" s="39"/>
+      <c r="F425" s="39"/>
+    </row>
+    <row r="426" spans="1:6" ht="60">
       <c r="A426" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B426" s="38" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="C426" s="41" t="s">
-        <v>661</v>
+        <v>586</v>
       </c>
       <c r="D426" s="38" t="s">
-        <v>579</v>
+        <v>1260</v>
       </c>
       <c r="E426" s="38"/>
       <c r="F426" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="427" spans="1:6">
+    <row r="427" spans="1:6" ht="30">
       <c r="A427" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B427" s="38" t="s">
-        <v>706</v>
-      </c>
-      <c r="C427" s="39" t="s">
-        <v>581</v>
-      </c>
-      <c r="D427" s="39"/>
-      <c r="E427" s="39"/>
-      <c r="F427" s="39"/>
-    </row>
-    <row r="428" spans="1:6" ht="90">
+        <v>709</v>
+      </c>
+      <c r="C427" s="41" t="s">
+        <v>710</v>
+      </c>
+      <c r="D427" s="38" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E427" s="38"/>
+      <c r="F427" s="38" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" ht="30">
       <c r="A428" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B428" s="38" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="C428" s="41" t="s">
-        <v>584</v>
+        <v>663</v>
       </c>
       <c r="D428" s="38" t="s">
-        <v>582</v>
+        <v>594</v>
       </c>
       <c r="E428" s="38"/>
       <c r="F428" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="429" spans="1:6" ht="60">
+    <row r="429" spans="1:6">
       <c r="A429" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B429" s="38" t="s">
-        <v>708</v>
-      </c>
-      <c r="C429" s="41" t="s">
-        <v>586</v>
-      </c>
-      <c r="D429" s="38" t="s">
-        <v>582</v>
-      </c>
-      <c r="E429" s="38"/>
-      <c r="F429" s="38" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="430" spans="1:6" ht="30">
+        <v>712</v>
+      </c>
+      <c r="C429" s="39" t="s">
+        <v>596</v>
+      </c>
+      <c r="D429" s="39"/>
+      <c r="E429" s="39"/>
+      <c r="F429" s="39"/>
+    </row>
+    <row r="430" spans="1:6">
       <c r="A430" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B430" s="38" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="C430" s="41" t="s">
-        <v>710</v>
+        <v>598</v>
       </c>
       <c r="D430" s="38" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="E430" s="38"/>
       <c r="F430" s="38" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="30">
+    <row r="431" spans="1:6">
       <c r="A431" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B431" s="38" t="s">
-        <v>711</v>
-      </c>
-      <c r="C431" s="41" t="s">
-        <v>663</v>
+        <v>714</v>
+      </c>
+      <c r="C431" s="38" t="s">
+        <v>600</v>
       </c>
       <c r="D431" s="38" t="s">
-        <v>594</v>
+        <v>1059</v>
       </c>
       <c r="E431" s="38"/>
       <c r="F431" s="38" t="s">
@@ -15490,27 +15504,27 @@
         <v>56</v>
       </c>
       <c r="B432" s="38" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="C432" s="39" t="s">
-        <v>596</v>
+        <v>1069</v>
       </c>
       <c r="D432" s="39"/>
       <c r="E432" s="39"/>
       <c r="F432" s="39"/>
     </row>
-    <row r="433" spans="1:6">
+    <row r="433" spans="1:6" ht="30">
       <c r="A433" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B433" s="38" t="s">
-        <v>713</v>
-      </c>
-      <c r="C433" s="41" t="s">
-        <v>598</v>
+        <v>720</v>
+      </c>
+      <c r="C433" s="38" t="s">
+        <v>611</v>
       </c>
       <c r="D433" s="38" t="s">
-        <v>573</v>
+        <v>1060</v>
       </c>
       <c r="E433" s="38"/>
       <c r="F433" s="38" t="s">
@@ -15521,48 +15535,44 @@
       <c r="A434" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B434" s="38" t="s">
-        <v>714</v>
-      </c>
-      <c r="C434" s="38" t="s">
-        <v>600</v>
-      </c>
-      <c r="D434" s="38" t="s">
-        <v>1059</v>
-      </c>
-      <c r="E434" s="38"/>
-      <c r="F434" s="38" t="s">
-        <v>1143</v>
-      </c>
+      <c r="B434" s="38">
+        <v>11.5</v>
+      </c>
+      <c r="C434" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D434" s="39"/>
+      <c r="E434" s="39"/>
+      <c r="F434" s="39"/>
     </row>
     <row r="435" spans="1:6">
       <c r="A435" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B435" s="38" t="s">
-        <v>715</v>
-      </c>
-      <c r="C435" s="39" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D435" s="39"/>
-      <c r="E435" s="39"/>
-      <c r="F435" s="39"/>
-    </row>
-    <row r="436" spans="1:6" ht="30">
+        <v>721</v>
+      </c>
+      <c r="C435" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D435" s="38"/>
+      <c r="E435" s="41"/>
+      <c r="F435" s="38" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6">
       <c r="A436" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B436" s="38" t="s">
-        <v>720</v>
-      </c>
-      <c r="C436" s="38" t="s">
-        <v>611</v>
-      </c>
-      <c r="D436" s="38" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E436" s="38"/>
+        <v>722</v>
+      </c>
+      <c r="C436" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D436" s="38"/>
+      <c r="E436" s="41"/>
       <c r="F436" s="38" t="s">
         <v>1143</v>
       </c>
@@ -15571,41 +15581,41 @@
       <c r="A437" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B437" s="38">
-        <v>11.5</v>
-      </c>
-      <c r="C437" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D437" s="39"/>
-      <c r="E437" s="39"/>
-      <c r="F437" s="39"/>
+      <c r="B437" s="38" t="s">
+        <v>723</v>
+      </c>
+      <c r="C437" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D437" s="38"/>
+      <c r="E437" s="41"/>
+      <c r="F437" s="38" t="s">
+        <v>1143</v>
+      </c>
     </row>
     <row r="438" spans="1:6">
       <c r="A438" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B438" s="38" t="s">
-        <v>721</v>
-      </c>
-      <c r="C438" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D438" s="38"/>
-      <c r="E438" s="41"/>
-      <c r="F438" s="38" t="s">
-        <v>1143</v>
-      </c>
+      <c r="B438" s="38">
+        <v>11.6</v>
+      </c>
+      <c r="C438" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D438" s="39"/>
+      <c r="E438" s="37"/>
+      <c r="F438" s="39"/>
     </row>
     <row r="439" spans="1:6">
       <c r="A439" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B439" s="38" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C439" s="41" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D439" s="38"/>
       <c r="E439" s="41"/>
@@ -15618,10 +15628,10 @@
         <v>56</v>
       </c>
       <c r="B440" s="38" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C440" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D440" s="38"/>
       <c r="E440" s="41"/>
@@ -15634,13 +15644,13 @@
         <v>56</v>
       </c>
       <c r="B441" s="38">
-        <v>11.6</v>
+        <v>11.7</v>
       </c>
       <c r="C441" s="37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D441" s="39"/>
-      <c r="E441" s="37"/>
+      <c r="E441" s="39"/>
       <c r="F441" s="39"/>
     </row>
     <row r="442" spans="1:6">
@@ -15648,109 +15658,109 @@
         <v>56</v>
       </c>
       <c r="B442" s="38" t="s">
-        <v>724</v>
-      </c>
-      <c r="C442" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="D442" s="38"/>
-      <c r="E442" s="41"/>
-      <c r="F442" s="38" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="443" spans="1:6">
+        <v>726</v>
+      </c>
+      <c r="C442" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D442" s="39"/>
+      <c r="E442" s="39"/>
+      <c r="F442" s="39"/>
+    </row>
+    <row r="443" spans="1:6" ht="105">
       <c r="A443" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B443" s="38" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C443" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D443" s="38"/>
-      <c r="E443" s="41"/>
+        <v>646</v>
+      </c>
+      <c r="D443" s="38">
+        <v>78.3</v>
+      </c>
+      <c r="E443" s="38"/>
       <c r="F443" s="38" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="444" spans="1:6">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" ht="30">
       <c r="A444" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B444" s="38">
-        <v>11.7</v>
-      </c>
-      <c r="C444" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D444" s="39"/>
-      <c r="E444" s="39"/>
-      <c r="F444" s="39"/>
-    </row>
-    <row r="445" spans="1:6">
+      <c r="B444" s="38" t="s">
+        <v>728</v>
+      </c>
+      <c r="C444" s="41" t="s">
+        <v>677</v>
+      </c>
+      <c r="D444" s="38">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E444" s="38"/>
+      <c r="F444" s="38" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" ht="30">
       <c r="A445" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B445" s="38" t="s">
-        <v>726</v>
-      </c>
-      <c r="C445" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D445" s="39"/>
-      <c r="E445" s="39"/>
-      <c r="F445" s="39"/>
-    </row>
-    <row r="446" spans="1:6" ht="105">
+        <v>729</v>
+      </c>
+      <c r="C445" s="41" t="s">
+        <v>650</v>
+      </c>
+      <c r="D445" s="38">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E445" s="38"/>
+      <c r="F445" s="38" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6">
       <c r="A446" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B446" s="38" t="s">
-        <v>727</v>
-      </c>
-      <c r="C446" s="41" t="s">
-        <v>646</v>
-      </c>
-      <c r="D446" s="38">
-        <v>78.3</v>
-      </c>
-      <c r="E446" s="38"/>
-      <c r="F446" s="38" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="447" spans="1:6" ht="30">
+        <v>730</v>
+      </c>
+      <c r="C446" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D446" s="39"/>
+      <c r="E446" s="39"/>
+      <c r="F446" s="39"/>
+    </row>
+    <row r="447" spans="1:6">
       <c r="A447" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B447" s="38" t="s">
-        <v>728</v>
-      </c>
-      <c r="C447" s="41" t="s">
-        <v>677</v>
-      </c>
-      <c r="D447" s="38">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E447" s="38"/>
-      <c r="F447" s="38" t="s">
-        <v>1087</v>
-      </c>
+        <v>731</v>
+      </c>
+      <c r="C447" s="39" t="s">
+        <v>619</v>
+      </c>
+      <c r="D447" s="39"/>
+      <c r="E447" s="39"/>
+      <c r="F447" s="39"/>
     </row>
     <row r="448" spans="1:6" ht="30">
       <c r="A448" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B448" s="38" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="C448" s="41" t="s">
-        <v>650</v>
-      </c>
-      <c r="D448" s="38">
-        <v>78.099999999999994</v>
+        <v>733</v>
+      </c>
+      <c r="D448" s="38" t="s">
+        <v>553</v>
       </c>
       <c r="E448" s="38"/>
       <c r="F448" s="38" t="s">
@@ -15762,41 +15772,49 @@
         <v>56</v>
       </c>
       <c r="B449" s="38" t="s">
-        <v>730</v>
-      </c>
-      <c r="C449" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D449" s="39"/>
-      <c r="E449" s="39"/>
-      <c r="F449" s="39"/>
-    </row>
-    <row r="450" spans="1:6">
+        <v>734</v>
+      </c>
+      <c r="C449" s="41" t="s">
+        <v>685</v>
+      </c>
+      <c r="D449" s="38" t="s">
+        <v>556</v>
+      </c>
+      <c r="E449" s="38"/>
+      <c r="F449" s="38" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" ht="30">
       <c r="A450" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B450" s="38" t="s">
-        <v>731</v>
-      </c>
-      <c r="C450" s="39" t="s">
-        <v>619</v>
-      </c>
-      <c r="D450" s="39"/>
-      <c r="E450" s="39"/>
-      <c r="F450" s="39"/>
-    </row>
-    <row r="451" spans="1:6" ht="30">
+        <v>735</v>
+      </c>
+      <c r="C450" s="38" t="s">
+        <v>736</v>
+      </c>
+      <c r="D450" s="38" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E450" s="38"/>
+      <c r="F450" s="38" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" ht="45">
       <c r="A451" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B451" s="38" t="s">
-        <v>732</v>
-      </c>
-      <c r="C451" s="41" t="s">
-        <v>733</v>
+        <v>737</v>
+      </c>
+      <c r="C451" s="38" t="s">
+        <v>738</v>
       </c>
       <c r="D451" s="38" t="s">
-        <v>553</v>
+        <v>594</v>
       </c>
       <c r="E451" s="38"/>
       <c r="F451" s="38" t="s">
@@ -15808,49 +15826,47 @@
         <v>56</v>
       </c>
       <c r="B452" s="38" t="s">
-        <v>734</v>
-      </c>
-      <c r="C452" s="41" t="s">
-        <v>685</v>
-      </c>
-      <c r="D452" s="38" t="s">
-        <v>556</v>
-      </c>
+        <v>739</v>
+      </c>
+      <c r="C452" s="38" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D452" s="38"/>
       <c r="E452" s="38"/>
       <c r="F452" s="38" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="453" spans="1:6" ht="30">
+    <row r="453" spans="1:6" ht="60">
       <c r="A453" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B453" s="38" t="s">
-        <v>735</v>
+        <v>1077</v>
       </c>
       <c r="C453" s="38" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="D453" s="38" t="s">
-        <v>1061</v>
+        <v>562</v>
       </c>
       <c r="E453" s="38"/>
       <c r="F453" s="38" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="454" spans="1:6" ht="45">
+    <row r="454" spans="1:6" ht="30">
       <c r="A454" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B454" s="38" t="s">
-        <v>737</v>
+        <v>1078</v>
       </c>
       <c r="C454" s="38" t="s">
-        <v>738</v>
+        <v>1075</v>
       </c>
       <c r="D454" s="38" t="s">
-        <v>594</v>
+        <v>695</v>
       </c>
       <c r="E454" s="38"/>
       <c r="F454" s="38" t="s">
@@ -15862,47 +15878,45 @@
         <v>56</v>
       </c>
       <c r="B455" s="38" t="s">
-        <v>739</v>
-      </c>
-      <c r="C455" s="38" t="s">
-        <v>1076</v>
-      </c>
-      <c r="D455" s="38"/>
-      <c r="E455" s="38"/>
-      <c r="F455" s="38" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="456" spans="1:6" ht="60">
+        <v>742</v>
+      </c>
+      <c r="C455" s="39" t="s">
+        <v>596</v>
+      </c>
+      <c r="D455" s="39"/>
+      <c r="E455" s="39"/>
+      <c r="F455" s="39"/>
+    </row>
+    <row r="456" spans="1:6">
       <c r="A456" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B456" s="38" t="s">
-        <v>1077</v>
-      </c>
-      <c r="C456" s="38" t="s">
-        <v>740</v>
+        <v>743</v>
+      </c>
+      <c r="C456" s="41" t="s">
+        <v>598</v>
       </c>
       <c r="D456" s="38" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="E456" s="38"/>
       <c r="F456" s="38" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="457" spans="1:6" ht="30">
+    <row r="457" spans="1:6">
       <c r="A457" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B457" s="38" t="s">
-        <v>1078</v>
+        <v>744</v>
       </c>
       <c r="C457" s="38" t="s">
-        <v>1075</v>
+        <v>600</v>
       </c>
       <c r="D457" s="38" t="s">
-        <v>695</v>
+        <v>1059</v>
       </c>
       <c r="E457" s="38"/>
       <c r="F457" s="38" t="s">
@@ -15914,10 +15928,10 @@
         <v>56</v>
       </c>
       <c r="B458" s="38" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="C458" s="39" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="D458" s="39"/>
       <c r="E458" s="39"/>
@@ -15928,63 +15942,67 @@
         <v>56</v>
       </c>
       <c r="B459" s="38" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="C459" s="41" t="s">
-        <v>598</v>
+        <v>566</v>
       </c>
       <c r="D459" s="38" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="E459" s="38"/>
       <c r="F459" s="38" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="460" spans="1:6">
+    <row r="460" spans="1:6" ht="30">
       <c r="A460" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B460" s="38" t="s">
-        <v>744</v>
-      </c>
-      <c r="C460" s="38" t="s">
-        <v>600</v>
+        <v>747</v>
+      </c>
+      <c r="C460" s="41" t="s">
+        <v>640</v>
       </c>
       <c r="D460" s="38" t="s">
-        <v>1059</v>
+        <v>570</v>
       </c>
       <c r="E460" s="38"/>
       <c r="F460" s="38" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="461" spans="1:6">
+    <row r="461" spans="1:6" ht="30">
       <c r="A461" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B461" s="38" t="s">
-        <v>745</v>
-      </c>
-      <c r="C461" s="39" t="s">
-        <v>602</v>
-      </c>
-      <c r="D461" s="39"/>
-      <c r="E461" s="39"/>
-      <c r="F461" s="39"/>
+        <v>748</v>
+      </c>
+      <c r="C461" s="41" t="s">
+        <v>607</v>
+      </c>
+      <c r="D461" s="38" t="s">
+        <v>573</v>
+      </c>
+      <c r="E461" s="38"/>
+      <c r="F461" s="38" t="s">
+        <v>1087</v>
+      </c>
     </row>
     <row r="462" spans="1:6">
       <c r="A462" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B462" s="38" t="s">
-        <v>746</v>
-      </c>
-      <c r="C462" s="41" t="s">
-        <v>566</v>
+        <v>749</v>
+      </c>
+      <c r="C462" s="38" t="s">
+        <v>609</v>
       </c>
       <c r="D462" s="38" t="s">
-        <v>567</v>
+        <v>1062</v>
       </c>
       <c r="E462" s="38"/>
       <c r="F462" s="38" t="s">
@@ -15996,70 +16014,16 @@
         <v>56</v>
       </c>
       <c r="B463" s="38" t="s">
-        <v>747</v>
-      </c>
-      <c r="C463" s="41" t="s">
-        <v>640</v>
+        <v>1259</v>
+      </c>
+      <c r="C463" s="38" t="s">
+        <v>611</v>
       </c>
       <c r="D463" s="38" t="s">
-        <v>570</v>
+        <v>1060</v>
       </c>
       <c r="E463" s="38"/>
       <c r="F463" s="38" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="464" spans="1:6" ht="30">
-      <c r="A464" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B464" s="38" t="s">
-        <v>748</v>
-      </c>
-      <c r="C464" s="41" t="s">
-        <v>607</v>
-      </c>
-      <c r="D464" s="38" t="s">
-        <v>573</v>
-      </c>
-      <c r="E464" s="38"/>
-      <c r="F464" s="38" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="465" spans="1:6">
-      <c r="A465" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B465" s="38" t="s">
-        <v>749</v>
-      </c>
-      <c r="C465" s="38" t="s">
-        <v>609</v>
-      </c>
-      <c r="D465" s="38" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E465" s="38"/>
-      <c r="F465" s="38" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="466" spans="1:6" ht="30">
-      <c r="A466" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B466" s="38" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C466" s="38" t="s">
-        <v>611</v>
-      </c>
-      <c r="D466" s="38" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E466" s="38"/>
-      <c r="F466" s="38" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -19475,10 +19439,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:IV27"/>
+  <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -21520,6 +21484,40 @@
       <c r="IU27" s="31"/>
       <c r="IV27" s="31"/>
     </row>
+    <row r="28" spans="1:256" ht="60">
+      <c r="A28" s="67" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B28" s="67" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C28" s="67" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+    </row>
+    <row r="29" spans="1:256" ht="30">
+      <c r="A29" s="53" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B29" s="67" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>588</v>
+      </c>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Synchronized after update to test overview
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_Production_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_Production_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD34FE8C-0FDF-48E0-9DED-7D1CE09893B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A45518-D430-4FDC-84C9-0A855B7F4410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="6168" windowWidth="23064" windowHeight="6204" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="1267">
   <si>
     <t>Card Capabilities Container</t>
   </si>
@@ -3828,6 +3828,12 @@
   </si>
   <si>
     <t>The Agency Code, System Code, and Credential Number of the FASC-N are present. The credential series, individual credential issue, person identifier, organizational category, organizational identifier, and person/organization association category of the FASC-N are populated</t>
+  </si>
+  <si>
+    <t>2.16.840.1.101.3.6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.3.6.1.1.16.4</t>
   </si>
 </sst>
 </file>
@@ -4629,7 +4635,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F473"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -12760,7 +12766,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -15494,7 +15500,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16069,7 +16077,9 @@
       <c r="D29" s="26" t="s">
         <v>1111</v>
       </c>
-      <c r="E29" s="26"/>
+      <c r="E29" s="26" t="s">
+        <v>1265</v>
+      </c>
       <c r="F29" s="21" t="s">
         <v>683</v>
       </c>
@@ -16088,7 +16098,9 @@
       <c r="D30" s="26" t="s">
         <v>1114</v>
       </c>
-      <c r="E30" s="26"/>
+      <c r="E30" s="26" t="s">
+        <v>1266</v>
+      </c>
       <c r="F30" s="21" t="s">
         <v>683</v>
       </c>
@@ -16216,7 +16228,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Corrected parameters for CMS.6
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_Production_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_Production_Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A45518-D430-4FDC-84C9-0A855B7F4410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF89FA02-703A-40D4-9007-B46932E07DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="6168" windowWidth="23064" windowHeight="6204" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2784" yWindow="384" windowWidth="20220" windowHeight="11940" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="2" r:id="rId1"/>
@@ -3821,9 +3821,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.1,CARDHOLDER_FINGERPRINTS_OID:2.16.840.1.101.3.6.2,CARDHOLDER_FACIAL_IMAGE_OID:2.16.840.1.101.3.6.2,CARDHOLDER_IRIS_IMAGES_OID:2.16.840</t>
-  </si>
-  <si>
     <t>Tags 0x3E and 0xFE are present and follow tags  in that order</t>
   </si>
   <si>
@@ -3834,6 +3831,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 1.3.6.1.1.16.4</t>
+  </si>
+  <si>
+    <t>CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.1,CARDHOLDER_FINGERPRINTS_OID:2.16.840.1.101.3.6.2,CARDHOLDER_FACIAL_IMAGE_OID:2.16.840.1.101.3.6.2,CARDHOLDER_IRIS_IMAGES_OID:2.16.840.1.101.3.6.2</t>
   </si>
 </sst>
 </file>
@@ -5181,7 +5181,7 @@
         <v>1012</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="D31" s="37" t="s">
         <v>103</v>
@@ -13171,7 +13171,7 @@
         <v>709</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
@@ -14014,7 +14014,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:IV50"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15500,8 +15500,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15631,7 +15631,7 @@
         <v>880</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>1262</v>
+        <v>1266</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>683</v>
@@ -16078,7 +16078,7 @@
         <v>1111</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>683</v>
@@ -16099,7 +16099,7 @@
         <v>1114</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>683</v>
@@ -16228,7 +16228,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>